<commit_message>
all four Pseudocomponents updated using data from chemsep databse
</commit_message>
<xml_diff>
--- a/OM_Compound_Creation/PseudoProp.xlsx
+++ b/OM_Compound_Creation/PseudoProp.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\FSF-2020-OM-CrudeDistillation\OM_Compound_Creation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E37607D-A932-49DB-A89F-377E0B0F26B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D139958-E0D2-4726-8EEE-498774FB48EA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E76E8132-0A12-4BB3-98DF-2F4341A20EB1}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{E76E8132-0A12-4BB3-98DF-2F4341A20EB1}"/>
   </bookViews>
   <sheets>
     <sheet name="All" sheetId="1" r:id="rId1"/>
@@ -2748,8 +2748,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.22265288713910761"/>
-                  <c:y val="-0.67437627588218141"/>
+                  <c:x val="-0.2167621312529304"/>
+                  <c:y val="-0.68762808250663587"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -5183,6 +5183,57 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="4"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.12129702537182852"/>
+                  <c:y val="-0.13030621172353457"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>'P1'!$E$17:$E$67</c:f>
@@ -19834,7 +19885,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EFA8C80-EF74-4118-A0AA-D3A90C25CC7B}">
   <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
@@ -19967,10 +20018,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35A483D1-A3AE-4202-929C-85421BD9814F}">
-  <dimension ref="B1:P67"/>
+  <dimension ref="A1:P67"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O7" sqref="O7"/>
+      <selection activeCell="C66" sqref="C66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -20049,7 +20100,10 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>1</v>
+      </c>
       <c r="B17" s="4">
         <v>211.06299999999999</v>
       </c>
@@ -20075,7 +20129,10 @@
         <v>0.36063800000000001</v>
       </c>
     </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>2</v>
+      </c>
       <c r="B18" s="4">
         <v>213.80600000000001</v>
       </c>
@@ -20101,7 +20158,10 @@
         <v>0.36063800000000001</v>
       </c>
     </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>3</v>
+      </c>
       <c r="B19" s="4">
         <v>216.55</v>
       </c>
@@ -20127,7 +20187,10 @@
         <v>0.36063800000000001</v>
       </c>
     </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>4</v>
+      </c>
       <c r="B20" s="4">
         <v>219.29400000000001</v>
       </c>
@@ -20153,7 +20216,10 @@
         <v>0.36063800000000001</v>
       </c>
     </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>5</v>
+      </c>
       <c r="B21" s="4">
         <v>222.03800000000001</v>
       </c>
@@ -20179,7 +20245,10 @@
         <v>0.36063800000000001</v>
       </c>
     </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>6</v>
+      </c>
       <c r="B22" s="4">
         <v>224.78200000000001</v>
       </c>
@@ -20205,7 +20274,10 @@
         <v>0.36063800000000001</v>
       </c>
     </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>7</v>
+      </c>
       <c r="B23" s="4">
         <v>227.52500000000001</v>
       </c>
@@ -20231,7 +20303,10 @@
         <v>0.36063800000000001</v>
       </c>
     </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>8</v>
+      </c>
       <c r="B24" s="4">
         <v>230.26900000000001</v>
       </c>
@@ -20257,7 +20332,10 @@
         <v>0.36063800000000001</v>
       </c>
     </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>9</v>
+      </c>
       <c r="B25" s="4">
         <v>233.01300000000001</v>
       </c>
@@ -20283,7 +20361,10 @@
         <v>0.36063800000000001</v>
       </c>
     </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>10</v>
+      </c>
       <c r="B26" s="4">
         <v>235.75700000000001</v>
       </c>
@@ -20309,7 +20390,10 @@
         <v>0.36063800000000001</v>
       </c>
     </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>11</v>
+      </c>
       <c r="B27" s="4">
         <v>238.501</v>
       </c>
@@ -20335,7 +20419,10 @@
         <v>0.36063800000000001</v>
       </c>
     </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>12</v>
+      </c>
       <c r="B28" s="4">
         <v>241.245</v>
       </c>
@@ -20361,7 +20448,10 @@
         <v>0.36063800000000001</v>
       </c>
     </row>
-    <row r="29" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>13</v>
+      </c>
       <c r="B29" s="4">
         <v>243.988</v>
       </c>
@@ -20387,7 +20477,10 @@
         <v>0.36063800000000001</v>
       </c>
     </row>
-    <row r="30" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>14</v>
+      </c>
       <c r="B30" s="4">
         <v>246.732</v>
       </c>
@@ -20413,7 +20506,10 @@
         <v>0.36063800000000001</v>
       </c>
     </row>
-    <row r="31" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>15</v>
+      </c>
       <c r="B31" s="4">
         <v>249.476</v>
       </c>
@@ -20439,7 +20535,10 @@
         <v>0.36063800000000001</v>
       </c>
     </row>
-    <row r="32" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>16</v>
+      </c>
       <c r="B32" s="4">
         <v>252.22</v>
       </c>
@@ -20465,7 +20564,10 @@
         <v>0.36063800000000001</v>
       </c>
     </row>
-    <row r="33" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>17</v>
+      </c>
       <c r="B33" s="4">
         <v>254.964</v>
       </c>
@@ -20491,7 +20593,10 @@
         <v>0.36063800000000001</v>
       </c>
     </row>
-    <row r="34" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>18</v>
+      </c>
       <c r="B34" s="4">
         <v>257.70699999999999</v>
       </c>
@@ -20517,7 +20622,10 @@
         <v>0.36063800000000001</v>
       </c>
     </row>
-    <row r="35" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>19</v>
+      </c>
       <c r="B35" s="4">
         <v>260.45100000000002</v>
       </c>
@@ -20543,7 +20651,10 @@
         <v>0.36063800000000001</v>
       </c>
     </row>
-    <row r="36" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>20</v>
+      </c>
       <c r="B36" s="4">
         <v>263.19499999999999</v>
       </c>
@@ -20569,7 +20680,10 @@
         <v>0.36063800000000001</v>
       </c>
     </row>
-    <row r="37" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>21</v>
+      </c>
       <c r="B37" s="4">
         <v>265.93900000000002</v>
       </c>
@@ -20595,7 +20709,10 @@
         <v>0.36063800000000001</v>
       </c>
     </row>
-    <row r="38" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>22</v>
+      </c>
       <c r="B38" s="4">
         <v>268.68299999999999</v>
       </c>
@@ -20621,7 +20738,10 @@
         <v>0.36063800000000001</v>
       </c>
     </row>
-    <row r="39" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>23</v>
+      </c>
       <c r="B39" s="4">
         <v>271.42700000000002</v>
       </c>
@@ -20647,7 +20767,10 @@
         <v>0.36063800000000001</v>
       </c>
     </row>
-    <row r="40" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>24</v>
+      </c>
       <c r="B40" s="4">
         <v>274.17</v>
       </c>
@@ -20673,7 +20796,10 @@
         <v>0.36063800000000001</v>
       </c>
     </row>
-    <row r="41" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>25</v>
+      </c>
       <c r="B41" s="4">
         <v>276.91399999999999</v>
       </c>
@@ -20699,7 +20825,10 @@
         <v>0.36063800000000001</v>
       </c>
     </row>
-    <row r="42" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>26</v>
+      </c>
       <c r="B42" s="4">
         <v>279.65800000000002</v>
       </c>
@@ -20725,7 +20854,10 @@
         <v>0.36063800000000001</v>
       </c>
     </row>
-    <row r="43" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>27</v>
+      </c>
       <c r="B43" s="4">
         <v>282.40199999999999</v>
       </c>
@@ -20751,7 +20883,10 @@
         <v>0.36063800000000001</v>
       </c>
     </row>
-    <row r="44" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>28</v>
+      </c>
       <c r="B44" s="4">
         <v>285.14600000000002</v>
       </c>
@@ -20777,7 +20912,10 @@
         <v>0.36063800000000001</v>
       </c>
     </row>
-    <row r="45" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>29</v>
+      </c>
       <c r="B45" s="4">
         <v>287.88900000000001</v>
       </c>
@@ -20803,7 +20941,10 @@
         <v>0.36063800000000001</v>
       </c>
     </row>
-    <row r="46" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>30</v>
+      </c>
       <c r="B46" s="4">
         <v>290.63299999999998</v>
       </c>
@@ -20829,7 +20970,10 @@
         <v>0.36063800000000001</v>
       </c>
     </row>
-    <row r="47" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>31</v>
+      </c>
       <c r="B47" s="4">
         <v>293.37700000000001</v>
       </c>
@@ -20855,7 +20999,10 @@
         <v>0.36063800000000001</v>
       </c>
     </row>
-    <row r="48" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>32</v>
+      </c>
       <c r="B48" s="4">
         <v>296.12099999999998</v>
       </c>
@@ -20881,7 +21028,10 @@
         <v>0.36063800000000001</v>
       </c>
     </row>
-    <row r="49" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>33</v>
+      </c>
       <c r="B49" s="4">
         <v>298.86500000000001</v>
       </c>
@@ -20907,7 +21057,10 @@
         <v>0.36063800000000001</v>
       </c>
     </row>
-    <row r="50" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>34</v>
+      </c>
       <c r="B50" s="4">
         <v>301.608</v>
       </c>
@@ -20933,7 +21086,10 @@
         <v>0.36063800000000001</v>
       </c>
     </row>
-    <row r="51" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>35</v>
+      </c>
       <c r="B51" s="4">
         <v>304.35199999999998</v>
       </c>
@@ -20959,7 +21115,10 @@
         <v>0.36063800000000001</v>
       </c>
     </row>
-    <row r="52" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>36</v>
+      </c>
       <c r="B52" s="4">
         <v>307.096</v>
       </c>
@@ -20985,7 +21144,10 @@
         <v>0.36063800000000001</v>
       </c>
     </row>
-    <row r="53" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <v>37</v>
+      </c>
       <c r="B53" s="4">
         <v>309.83999999999997</v>
       </c>
@@ -21011,7 +21173,10 @@
         <v>0.36063800000000001</v>
       </c>
     </row>
-    <row r="54" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <v>38</v>
+      </c>
       <c r="B54" s="4">
         <v>312.584</v>
       </c>
@@ -21037,7 +21202,10 @@
         <v>0.36063800000000001</v>
       </c>
     </row>
-    <row r="55" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <v>39</v>
+      </c>
       <c r="B55" s="4">
         <v>315.32799999999997</v>
       </c>
@@ -21063,7 +21231,10 @@
         <v>0.36063800000000001</v>
       </c>
     </row>
-    <row r="56" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <v>40</v>
+      </c>
       <c r="B56" s="4">
         <v>318.07100000000003</v>
       </c>
@@ -21089,7 +21260,10 @@
         <v>0.36063800000000001</v>
       </c>
     </row>
-    <row r="57" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A57">
+        <v>41</v>
+      </c>
       <c r="B57" s="4">
         <v>320.815</v>
       </c>
@@ -21115,7 +21289,10 @@
         <v>0.36063800000000001</v>
       </c>
     </row>
-    <row r="58" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A58">
+        <v>42</v>
+      </c>
       <c r="B58" s="4">
         <v>323.55900000000003</v>
       </c>
@@ -21141,7 +21318,10 @@
         <v>0.36063800000000001</v>
       </c>
     </row>
-    <row r="59" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A59">
+        <v>43</v>
+      </c>
       <c r="B59" s="4">
         <v>326.303</v>
       </c>
@@ -21167,7 +21347,10 @@
         <v>0.36063800000000001</v>
       </c>
     </row>
-    <row r="60" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A60">
+        <v>44</v>
+      </c>
       <c r="B60" s="4">
         <v>329.04700000000003</v>
       </c>
@@ -21193,7 +21376,10 @@
         <v>0.36063800000000001</v>
       </c>
     </row>
-    <row r="61" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A61">
+        <v>45</v>
+      </c>
       <c r="B61" s="4">
         <v>331.79</v>
       </c>
@@ -21219,7 +21405,10 @@
         <v>0.36063800000000001</v>
       </c>
     </row>
-    <row r="62" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A62">
+        <v>46</v>
+      </c>
       <c r="B62" s="4">
         <v>334.53399999999999</v>
       </c>
@@ -21245,7 +21434,10 @@
         <v>0.36063800000000001</v>
       </c>
     </row>
-    <row r="63" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A63">
+        <v>47</v>
+      </c>
       <c r="B63" s="4">
         <v>337.27800000000002</v>
       </c>
@@ -21271,7 +21463,10 @@
         <v>0.36063800000000001</v>
       </c>
     </row>
-    <row r="64" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A64">
+        <v>48</v>
+      </c>
       <c r="B64" s="4">
         <v>340.02199999999999</v>
       </c>
@@ -21297,7 +21492,10 @@
         <v>0.36063800000000001</v>
       </c>
     </row>
-    <row r="65" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A65">
+        <v>49</v>
+      </c>
       <c r="B65" s="4">
         <v>342.76600000000002</v>
       </c>
@@ -21323,7 +21521,10 @@
         <v>0.36063800000000001</v>
       </c>
     </row>
-    <row r="66" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A66">
+        <v>50</v>
+      </c>
       <c r="B66" s="4">
         <v>345.50900000000001</v>
       </c>
@@ -21349,7 +21550,10 @@
         <v>0.36063800000000001</v>
       </c>
     </row>
-    <row r="67" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A67">
+        <v>51</v>
+      </c>
       <c r="B67" s="4">
         <v>348.25299999999999</v>
       </c>
@@ -22806,8 +23010,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{434EB6DF-BC62-419D-B435-F69031383F14}">
   <dimension ref="B1:P67"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -24226,7 +24430,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DF039BF-BB01-4E6A-8C3C-004AA3DD5F84}">
   <dimension ref="B1:P67"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>

</xml_diff>